<commit_message>
Revert "small updates (?)"
This reverts commit 221cb2ef10fc30988aeb9e8a239a4ffcd3e23b9a.
</commit_message>
<xml_diff>
--- a/Interview small data.xlsx
+++ b/Interview small data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/darryl_teo_sutd_edu_sg/Documents/Desktop/SUTD/NOT so SUTD/job/CV resume apps/2025-10 application htx/Technical-Test---Tutor-Student-Matching-Problem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/darryl_teo_mymail_sutd_edu_sg/Documents/Desktop/SUTD/NOT so SUTD/job/CV resume etc/2025-10 application htx/Technical-Test---Tutor-Student-Matching-Problem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{D54AC2EF-5E58-4430-80C4-E8F45C2C7413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76AC6C80-A2CE-442A-9F9A-8EEA913FD6CF}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{D54AC2EF-5E58-4430-80C4-E8F45C2C7413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E23CB02C-A9BF-4E3C-89A8-0BB444FCA178}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="771" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="771" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Students" sheetId="1" r:id="rId1"/>
@@ -1291,10 +1291,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1658C2E9-992B-45F8-A677-52782C4638AC}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A38" sqref="A38:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,7 +1323,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -1390,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -1560,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>117</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -1696,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -1713,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -1747,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>117</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>117</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>117</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -1900,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>117</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>117</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -2036,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>117</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>117</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>119</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>119</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -2240,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -2257,7 +2258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -2274,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -2342,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>119</v>
       </c>
@@ -2393,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>119</v>
       </c>
@@ -2444,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>119</v>
       </c>
@@ -2563,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>119</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>122</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>122</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>122</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>122</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>122</v>
       </c>
@@ -2665,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>122</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>122</v>
       </c>
@@ -2699,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>122</v>
       </c>
@@ -2716,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>122</v>
       </c>
@@ -2733,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>122</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>122</v>
       </c>
@@ -2767,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>122</v>
       </c>
@@ -2784,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>122</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>122</v>
       </c>
@@ -2818,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>122</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>122</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>122</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>122</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>122</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>122</v>
       </c>
@@ -2937,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>122</v>
       </c>
@@ -2954,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>122</v>
       </c>
@@ -2971,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>122</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>122</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>122</v>
       </c>
@@ -3039,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>122</v>
       </c>
@@ -3073,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>122</v>
       </c>
@@ -3090,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -3108,7 +3109,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E106" xr:uid="{1658C2E9-992B-45F8-A677-52782C4638AC}"/>
+  <autoFilter ref="E1:E106" xr:uid="{1658C2E9-992B-45F8-A677-52782C4638AC}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>